<commit_message>
Greedy Backward completed, repository organized (2)
</commit_message>
<xml_diff>
--- a/results/Results_PCA.xlsx
+++ b/results/Results_PCA.xlsx
@@ -455,10 +455,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>5312.286249294629</v>
+        <v>5312.286275944365</v>
       </c>
       <c r="C2" t="n">
-        <v>5700.098211346549</v>
+        <v>5700.099400947533</v>
       </c>
       <c r="D2" t="n">
         <v>54.87311443662782</v>
@@ -469,10 +469,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>5312.273125953214</v>
+        <v>5312.273112865018</v>
       </c>
       <c r="C3" t="n">
-        <v>5700.466704314611</v>
+        <v>5700.466120521982</v>
       </c>
       <c r="D3" t="n">
         <v>74.15442319885639</v>
@@ -483,10 +483,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>5312.258455031836</v>
+        <v>5312.25843422957</v>
       </c>
       <c r="C4" t="n">
-        <v>5700.619466997397</v>
+        <v>5700.618543704751</v>
       </c>
       <c r="D4" t="n">
         <v>81.50751568500387</v>
@@ -497,10 +497,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>5311.972199052095</v>
+        <v>5311.972213691312</v>
       </c>
       <c r="C5" t="n">
-        <v>5703.321298448602</v>
+        <v>5703.321946459234</v>
       </c>
       <c r="D5" t="n">
         <v>87.82323973010362</v>
@@ -511,10 +511,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>5204.9868779012</v>
+        <v>5204.986866309459</v>
       </c>
       <c r="C6" t="n">
-        <v>5572.232223435005</v>
+        <v>5572.231769467213</v>
       </c>
       <c r="D6" t="n">
         <v>92.53980490726534</v>
@@ -525,10 +525,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>5204.940828717232</v>
+        <v>5204.940820156914</v>
       </c>
       <c r="C7" t="n">
-        <v>5571.237768165332</v>
+        <v>5571.237434935648</v>
       </c>
       <c r="D7" t="n">
         <v>95.68013994469391</v>
@@ -539,10 +539,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>5195.55306043967</v>
+        <v>5195.553024188598</v>
       </c>
       <c r="C8" t="n">
-        <v>5577.59778462348</v>
+        <v>5577.596446742497</v>
       </c>
       <c r="D8" t="n">
         <v>97.91331841817298</v>
@@ -553,10 +553,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>5195.350432160702</v>
+        <v>5195.350385791561</v>
       </c>
       <c r="C9" t="n">
-        <v>5578.424155882287</v>
+        <v>5578.422448175799</v>
       </c>
       <c r="D9" t="n">
         <v>98.44901646162687</v>
@@ -567,10 +567,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>5155.670297274284</v>
+        <v>5155.670286097942</v>
       </c>
       <c r="C10" t="n">
-        <v>5542.461807424918</v>
+        <v>5542.461420431901</v>
       </c>
       <c r="D10" t="n">
         <v>98.81189048295249</v>
@@ -581,10 +581,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>5079.480642622491</v>
+        <v>5079.480701206051</v>
       </c>
       <c r="C11" t="n">
-        <v>5464.110908567722</v>
+        <v>5464.112953638824</v>
       </c>
       <c r="D11" t="n">
         <v>99.16108462090826</v>
@@ -595,10 +595,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>5073.467457752922</v>
+        <v>5073.467434526081</v>
       </c>
       <c r="C12" t="n">
-        <v>5468.838634919656</v>
+        <v>5468.837813094297</v>
       </c>
       <c r="D12" t="n">
         <v>99.348554063284</v>
@@ -609,10 +609,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>4926.397883338807</v>
+        <v>4926.397885820033</v>
       </c>
       <c r="C13" t="n">
-        <v>5261.520717562425</v>
+        <v>5261.520809347274</v>
       </c>
       <c r="D13" t="n">
         <v>99.50793485783758</v>
@@ -623,10 +623,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>4926.37400945135</v>
+        <v>4926.374045778306</v>
       </c>
       <c r="C14" t="n">
-        <v>5262.159489747199</v>
+        <v>5262.16084025453</v>
       </c>
       <c r="D14" t="n">
         <v>99.63347501289206</v>
@@ -637,10 +637,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>4895.873274936752</v>
+        <v>4895.873226092914</v>
       </c>
       <c r="C15" t="n">
-        <v>5229.056227652545</v>
+        <v>5229.054412805319</v>
       </c>
       <c r="D15" t="n">
         <v>99.75331454877467</v>
@@ -651,10 +651,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>4878.227373718642</v>
+        <v>4878.227427266665</v>
       </c>
       <c r="C16" t="n">
-        <v>5229.476830978077</v>
+        <v>5229.478711918437</v>
       </c>
       <c r="D16" t="n">
         <v>99.81442911166806</v>
@@ -665,10 +665,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>4878.151206639959</v>
+        <v>4878.151146901041</v>
       </c>
       <c r="C17" t="n">
-        <v>5230.180710738043</v>
+        <v>5230.178599566806</v>
       </c>
       <c r="D17" t="n">
         <v>99.85729633389292</v>
@@ -679,10 +679,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>4877.964563159149</v>
+        <v>4877.964580016186</v>
       </c>
       <c r="C18" t="n">
-        <v>5231.897745276196</v>
+        <v>5231.898346024969</v>
       </c>
       <c r="D18" t="n">
         <v>99.89076672442093</v>
@@ -693,10 +693,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>4877.901948631218</v>
+        <v>4877.901910289549</v>
       </c>
       <c r="C19" t="n">
-        <v>5233.967105963961</v>
+        <v>5233.965739285173</v>
       </c>
       <c r="D19" t="n">
         <v>99.92015303083093</v>
@@ -707,10 +707,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>4776.070686559707</v>
+        <v>4776.070651716709</v>
       </c>
       <c r="C20" t="n">
-        <v>5135.388568356088</v>
+        <v>5135.387410419341</v>
       </c>
       <c r="D20" t="n">
         <v>99.94289275867352</v>
@@ -721,10 +721,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>4775.926798341738</v>
+        <v>4775.926817870442</v>
       </c>
       <c r="C21" t="n">
-        <v>5133.711305209534</v>
+        <v>5133.711954007724</v>
       </c>
       <c r="D21" t="n">
         <v>99.96188072660689</v>
@@ -735,10 +735,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>4753.471789958545</v>
+        <v>4753.47181185821</v>
       </c>
       <c r="C22" t="n">
-        <v>5085.099942938551</v>
+        <v>5085.100686932095</v>
       </c>
       <c r="D22" t="n">
         <v>99.97570180522541</v>
@@ -749,10 +749,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>4636.198556091445</v>
+        <v>4636.198576792334</v>
       </c>
       <c r="C23" t="n">
-        <v>5059.166680597362</v>
+        <v>5059.167304844145</v>
       </c>
       <c r="D23" t="n">
         <v>99.98574788042984</v>
@@ -763,10 +763,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>4604.103123376316</v>
+        <v>4604.103121611704</v>
       </c>
       <c r="C24" t="n">
-        <v>5032.138954184197</v>
+        <v>5032.138900976538</v>
       </c>
       <c r="D24" t="n">
         <v>99.99205319219433</v>
@@ -777,10 +777,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>4595.00958534608</v>
+        <v>4595.00958296953</v>
       </c>
       <c r="C25" t="n">
-        <v>5004.424405553797</v>
+        <v>5004.424335920257</v>
       </c>
       <c r="D25" t="n">
         <v>99.99664466405726</v>
@@ -791,10 +791,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>4593.350197080056</v>
+        <v>4593.350238470071</v>
       </c>
       <c r="C26" t="n">
-        <v>5002.510899263304</v>
+        <v>5002.512076745834</v>
       </c>
       <c r="D26" t="n">
         <v>99.99999999999996</v>
@@ -805,10 +805,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>4593.169092383298</v>
+        <v>4593.169147634101</v>
       </c>
       <c r="C27" t="n">
-        <v>5006.61040027981</v>
+        <v>5006.611977572868</v>
       </c>
       <c r="D27" t="n">
         <v>99.99999999999996</v>

</xml_diff>